<commit_message>
Adding couple of users to excel for testing
</commit_message>
<xml_diff>
--- a/database/employee_db.xlsx
+++ b/database/employee_db.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\2025\GTCI\BookYourMeal\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C4641EF-A3D1-4122-A414-3A8B1D446559}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1428341F-9FB8-4FD0-8302-A43457FE8C6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{21D1C28C-9FFF-4595-A1BF-CB15A039FE45}"/>
+    <workbookView xWindow="11496" yWindow="4572" windowWidth="14376" windowHeight="7260" xr2:uid="{21D1C28C-9FFF-4595-A1BF-CB15A039FE45}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
   <si>
     <t>K M Swaminadh</t>
   </si>
@@ -63,6 +63,21 @@
   </si>
   <si>
     <t>swamynadh.engg@gmail.com</t>
+  </si>
+  <si>
+    <t>Sakshi Jain</t>
+  </si>
+  <si>
+    <t>sakshi_jain@goodyear.com</t>
+  </si>
+  <si>
+    <t>Ammiraju Rajasekhar</t>
+  </si>
+  <si>
+    <t>ammiraju_rajasekhar@goodyear.com</t>
+  </si>
+  <si>
+    <t>AExxxxx</t>
   </si>
 </sst>
 </file>
@@ -445,19 +460,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{057A9B6B-B104-4BF2-B866-4A7CEE6FA0A7}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="23" customWidth="1"/>
-    <col min="3" max="3" width="30.7265625" customWidth="1"/>
+    <col min="3" max="3" width="30.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -468,32 +483,54 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B4" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C4" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
         <v>6</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B5" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C5" s="1" t="s">
         <v>8</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" xr:uid="{15CC67EA-B446-48DF-92D0-50DC16D88C1B}"/>
-    <hyperlink ref="C3" r:id="rId2" xr:uid="{62F9560E-662A-4481-A307-DEE301D079DE}"/>
+    <hyperlink ref="C4" r:id="rId1" xr:uid="{15CC67EA-B446-48DF-92D0-50DC16D88C1B}"/>
+    <hyperlink ref="C5" r:id="rId2" xr:uid="{62F9560E-662A-4481-A307-DEE301D079DE}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>